<commit_message>
Add test + Fix bug
</commit_message>
<xml_diff>
--- a/src/main/webapp/WEB-INF/data/TL_TRICKService_NormImport_V1.1.xlsx
+++ b/src/main/webapp/WEB-INF/data/TL_TRICKService_NormImport_V1.1.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="50">
   <si>
     <t>Name</t>
   </si>
@@ -126,12 +126,52 @@
   </si>
   <si>
     <t>sdfs</t>
+  </si>
+  <si>
+    <t>Standard for test</t>
+  </si>
+  <si>
+    <t>This standard for testing</t>
+  </si>
+  <si>
+    <t>Domain_ENG</t>
+  </si>
+  <si>
+    <t>Description_ENG</t>
+  </si>
+  <si>
+    <t>Domain_FRA</t>
+  </si>
+  <si>
+    <t>Description_FRA</t>
+  </si>
+  <si>
+    <t>Level 1 domain</t>
+  </si>
+  <si>
+    <t>Level 1 description</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>Level 2 domain</t>
+  </si>
+  <si>
+    <t>Level 2 description</t>
+  </si>
+  <si>
+    <t>Level 3 domain</t>
+  </si>
+  <si>
+    <t>Level 3 description</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="0"/>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -199,16 +239,13 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="TableNormData" displayName="TableNormData" ref="A1:G6" totalsRowShown="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="TableNormData" displayName="TableNormData" ref="A1:H4" totalsRowShown="0">
   <autoFilter ref="A1:G6"/>
   <tableColumns count="7">
-    <tableColumn id="1" name="Level"/>
-    <tableColumn id="2" name="Reference" dataDxfId="0"/>
-    <tableColumn id="5" name="Computable"/>
-    <tableColumn id="3" name="Domain_eng"/>
-    <tableColumn id="4" name="Description_eng"/>
-    <tableColumn id="6" name="Domain_fr"/>
-    <tableColumn id="7" name="Description_fr"/>
+    <tableColumn name="domain" id="4"/>
+    <tableColumn name="40" id="5"/>
+    <tableColumn name="41" id="6"/>
+    <tableColumn name="42" id="7"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -509,10 +546,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="8.42578125" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="10.0" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="14.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -531,13 +568,13 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B2">
-        <v>2014</v>
+        <v>37</v>
+      </c>
+      <c r="B2" t="n">
+        <v>2015.0</v>
       </c>
       <c r="C2" t="s">
-        <v>7</v>
+        <v>38</v>
       </c>
       <c r="D2" t="b">
         <v>1</v>
@@ -561,41 +598,41 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="7.85546875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="1" width="12.28515625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="14.0" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="14.28515625" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="17.7109375" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="13.42578125" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="16.85546875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="A1" t="s" s="0">
         <v>4</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="0" t="s">
         <v>5</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" t="s" s="0">
         <v>3</v>
       </c>
-      <c r="D1" t="s">
-        <v>21</v>
-      </c>
-      <c r="E1" t="s">
-        <v>22</v>
-      </c>
-      <c r="F1" t="s">
-        <v>19</v>
-      </c>
-      <c r="G1" t="s">
-        <v>20</v>
+      <c r="D1" t="s" s="0">
+        <v>39</v>
+      </c>
+      <c r="E1" t="s" s="0">
+        <v>40</v>
+      </c>
+      <c r="F1" t="s" s="0">
+        <v>41</v>
+      </c>
+      <c r="G1" t="s" s="0">
+        <v>42</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>1</v>
+      <c r="A2" t="n">
+        <v>1.0</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>24</v>
@@ -604,87 +641,65 @@
         <v>0</v>
       </c>
       <c r="D2" t="s">
-        <v>6</v>
+        <v>43</v>
       </c>
       <c r="E2" t="s">
-        <v>8</v>
+        <v>44</v>
       </c>
       <c r="F2" t="s">
-        <v>27</v>
+        <v>45</v>
       </c>
       <c r="G2" t="s">
-        <v>28</v>
+        <v>45</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3" s="1" t="s">
+    <row r="3">
+      <c r="A3" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="B3" t="s">
         <v>25</v>
       </c>
       <c r="C3" t="b">
         <v>0</v>
       </c>
       <c r="D3" t="s">
-        <v>11</v>
+        <v>46</v>
       </c>
       <c r="E3" t="s">
-        <v>15</v>
+        <v>47</v>
       </c>
       <c r="F3" t="s">
-        <v>29</v>
+        <v>45</v>
       </c>
       <c r="G3" t="s">
-        <v>30</v>
+        <v>45</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>3</v>
-      </c>
-      <c r="B4" s="1" t="s">
+    <row r="4">
+      <c r="A4" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="B4" t="s">
         <v>9</v>
       </c>
       <c r="C4" t="b">
         <v>1</v>
       </c>
       <c r="D4" t="s">
-        <v>12</v>
+        <v>48</v>
       </c>
       <c r="E4" t="s">
-        <v>16</v>
+        <v>49</v>
       </c>
       <c r="F4" t="s">
-        <v>31</v>
+        <v>45</v>
       </c>
       <c r="G4" t="s">
-        <v>36</v>
+        <v>45</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>2</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C5" t="b">
-        <v>0</v>
-      </c>
-      <c r="D5" t="s">
-        <v>13</v>
-      </c>
-      <c r="E5" t="s">
-        <v>17</v>
-      </c>
-      <c r="F5" t="s">
-        <v>32</v>
-      </c>
-      <c r="G5" t="s">
-        <v>33</v>
-      </c>
-    </row>
+    <row r="5"/>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>3</v>

</xml_diff>

<commit_message>
fix unit test (quantitative only)
</commit_message>
<xml_diff>
--- a/src/main/webapp/WEB-INF/data/TL_TRICKService_NormImport_V1.1.xlsx
+++ b/src/main/webapp/WEB-INF/data/TL_TRICKService_NormImport_V1.1.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="16925"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\eomar\Desktop\"/>
     </mc:Choice>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="27">
   <si>
     <t>Name</t>
   </si>
@@ -108,6 +108,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <numFmts count="0"/>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -178,16 +179,13 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:G6" totalsRowShown="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:H4" totalsRowShown="0">
   <autoFilter ref="A1:G6"/>
   <tableColumns count="7">
-    <tableColumn id="1" name="Level"/>
-    <tableColumn id="2" name="Reference" dataDxfId="0"/>
-    <tableColumn id="3" name="Computable"/>
-    <tableColumn id="4" name="Domain_ENG"/>
-    <tableColumn id="5" name="Description_ENG"/>
-    <tableColumn id="6" name="Domain_FRA"/>
-    <tableColumn id="7" name="Description_FRA"/>
+    <tableColumn name="domain" id="4"/>
+    <tableColumn name="17" id="5"/>
+    <tableColumn name="18" id="6"/>
+    <tableColumn name="19" id="7"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -522,10 +520,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="10" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="14" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="8.42578125" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="10.0" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="14.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -546,8 +544,8 @@
       <c r="A2" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B2">
-        <v>2015</v>
+      <c r="B2" t="n">
+        <v>2015.0</v>
       </c>
       <c r="C2" t="s">
         <v>15</v>
@@ -574,41 +572,41 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="12.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="14" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="14.85546875" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="18.140625" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="14.42578125" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="17.7109375" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="7.85546875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="1" width="12.28515625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="14.0" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="14.85546875" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="18.140625" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="14.42578125" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="17.7109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="A1" t="s" s="0">
         <v>4</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" t="s" s="0">
         <v>5</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" t="s" s="0">
         <v>3</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" t="s" s="0">
         <v>16</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" t="s" s="0">
         <v>17</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" t="s" s="0">
         <v>18</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" t="s" s="0">
         <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>1</v>
+      <c r="A2" t="n">
+        <v>1.0</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>10</v>
@@ -629,9 +627,9 @@
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>2</v>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>2.0</v>
       </c>
       <c r="B3" t="s">
         <v>11</v>
@@ -652,9 +650,9 @@
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>3</v>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>3.0</v>
       </c>
       <c r="B4" t="s">
         <v>6</v>
@@ -675,6 +673,7 @@
         <v>22</v>
       </c>
     </row>
+    <row r="5"/>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>3</v>

</xml_diff>

<commit_message>
Fix bug + update css
</commit_message>
<xml_diff>
--- a/src/main/webapp/WEB-INF/data/TL_TRICKService_NormImport_V1.1.xlsx
+++ b/src/main/webapp/WEB-INF/data/TL_TRICKService_NormImport_V1.1.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="16925"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent>
@@ -9,11 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="120" yWindow="15" windowWidth="28620" windowHeight="12915" activeTab="1"/>
+    <workbookView activeTab="1" windowHeight="12915" windowWidth="28620" xWindow="120" yWindow="15"/>
   </bookViews>
   <sheets>
-    <sheet name="NormInfo" sheetId="1" r:id="rId1"/>
-    <sheet name="NormData" sheetId="2" r:id="rId2"/>
+    <sheet name="NormInfo" r:id="rId1" sheetId="1"/>
+    <sheet name="NormData" r:id="rId2" sheetId="2"/>
   </sheets>
   <calcPr calcId="145621"/>
   <fileRecoveryPr repairLoad="1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="27">
   <si>
     <t>Name</t>
   </si>
@@ -136,24 +136,24 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
   </cellStyles>
   <dxfs count="2">
     <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
+      <numFmt formatCode="@" numFmtId="30"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
+      <numFmt formatCode="@" numFmtId="30"/>
     </dxf>
   </dxfs>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -166,20 +166,20 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="TableNormInfo" displayName="TableNormInfo" ref="A1:D2" totalsRowShown="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" displayName="TableNormInfo" id="1" name="TableNormInfo" ref="A1:D2" totalsRowShown="0">
   <autoFilter ref="A1:D2"/>
   <tableColumns count="4">
-    <tableColumn id="1" name="Name" dataDxfId="1"/>
+    <tableColumn dataDxfId="1" id="1" name="Name"/>
     <tableColumn id="2" name="Version"/>
     <tableColumn id="3" name="Description"/>
     <tableColumn id="4" name="Computable"/>
   </tableColumns>
-  <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+  <tableStyleInfo name="TableStyleMedium9" showColumnStripes="0" showFirstColumn="0" showLastColumn="0" showRowStripes="1"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:H4" totalsRowShown="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" displayName="Table2" id="2" name="Table2" ref="A1:H4" totalsRowShown="0">
   <autoFilter ref="A1:G6"/>
   <tableColumns count="7">
     <tableColumn name="domain" id="4"/>
@@ -187,7 +187,7 @@
     <tableColumn name="18" id="6"/>
     <tableColumn name="19" id="7"/>
   </tableColumns>
-  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+  <tableStyleInfo name="TableStyleMedium2" showColumnStripes="0" showFirstColumn="0" showLastColumn="0" showRowStripes="1"/>
 </table>
 </file>
 
@@ -196,10 +196,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr lastClr="000000" val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -234,7 +234,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin panose="020F0302020204030204" typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -286,7 +286,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin panose="020F0502020204030204" typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -391,7 +391,7 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="9525">
           <a:solidFill>
             <a:schemeClr val="phClr">
               <a:shade val="95000"/>
@@ -400,13 +400,13 @@
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="25400">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="38100">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -416,7 +416,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dir="5400000" dist="20000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -425,7 +425,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dir="5400000" dist="23000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -434,7 +434,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dir="5400000" dist="23000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -444,12 +444,12 @@
             <a:camera prst="orthographicFront">
               <a:rot lat="0" lon="0" rev="0"/>
             </a:camera>
-            <a:lightRig rig="threePt" dir="t">
+            <a:lightRig dir="t" rig="threePt">
               <a:rot lat="0" lon="0" rev="1200000"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
-            <a:bevelT w="63500" h="25400"/>
+            <a:bevelT h="25400" w="63500"/>
           </a:sp3d>
         </a:effectStyle>
       </a:effectStyleLst>
@@ -480,7 +480,7 @@
             </a:gs>
           </a:gsLst>
           <a:path path="circle">
-            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+            <a:fillToRect b="180000" l="50000" r="50000" t="-80000"/>
           </a:path>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
@@ -499,7 +499,7 @@
             </a:gs>
           </a:gsLst>
           <a:path path="circle">
-            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+            <a:fillToRect b="50000" l="50000" r="50000" t="50000"/>
           </a:path>
         </a:gradFill>
       </a:bgFillStyleLst>
@@ -511,7 +511,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -555,7 +555,7 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <tableParts count="1">
     <tablePart r:id="rId1"/>
   </tableParts>
@@ -563,7 +563,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
@@ -582,25 +582,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" t="s" s="0">
+      <c r="A1" s="0" t="s">
         <v>4</v>
       </c>
-      <c r="B1" t="s" s="0">
+      <c r="B1" s="0" t="s">
         <v>5</v>
       </c>
-      <c r="C1" t="s" s="0">
+      <c r="C1" s="0" t="s">
         <v>3</v>
       </c>
-      <c r="D1" t="s" s="0">
+      <c r="D1" s="0" t="s">
         <v>16</v>
       </c>
-      <c r="E1" t="s" s="0">
+      <c r="E1" s="0" t="s">
         <v>17</v>
       </c>
-      <c r="F1" t="s" s="0">
+      <c r="F1" s="0" t="s">
         <v>18</v>
       </c>
-      <c r="G1" t="s" s="0">
+      <c r="G1" s="0" t="s">
         <v>19</v>
       </c>
     </row>
@@ -698,8 +698,8 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup horizontalDpi="0" orientation="portrait" paperSize="9" r:id="rId1" verticalDpi="0"/>
   <tableParts count="1">
     <tablePart r:id="rId2"/>
   </tableParts>

</xml_diff>